<commit_message>
aber bitte nicht so schnell
</commit_message>
<xml_diff>
--- a/B 2.2/Messdaten/Auswertungsskripte/B2.2.xlsx
+++ b/B 2.2/Messdaten/Auswertungsskripte/B2.2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesco\Documents\Praktikum-test\B 2.2\Messdaten\Auswertungsskripte\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dtimo\Desktop\Praktikum\praktikum\B 2.2\Messdaten\Auswertungsskripte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461EFF26-93E8-4EEA-BB25-8449F42FA778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209F8386-F17F-4440-9914-DD2BD0AB645C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -180,7 +180,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,6 +205,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -218,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -232,6 +238,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -514,7 +521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:BA57"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -3060,8 +3067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{540561B1-14D7-4856-AC05-2802599319CD}">
   <dimension ref="B4:X68"/>
   <sheetViews>
-    <sheetView topLeftCell="B43" workbookViewId="0">
-      <selection activeCell="J68" sqref="J68"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="O55" sqref="O55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4982,6 +4989,10 @@
         <f>AVERAGE(L51:M51,P51:Q51,S51:T51,W51)</f>
         <v>0.38727533215341853</v>
       </c>
+      <c r="M53" s="9">
+        <f>AVERAGE(L51:M51,P51:Q51,S51:T51)</f>
+        <v>0.17569823989767314</v>
+      </c>
     </row>
     <row r="54" spans="2:24" x14ac:dyDescent="0.25">
       <c r="K54" t="s">
@@ -4990,6 +5001,10 @@
       <c r="L54">
         <f>SQRT(1/30*SUM(L52:M52,P52,Q52,S52,W52))</f>
         <v>0.21618140767867511</v>
+      </c>
+      <c r="M54" s="9">
+        <f>SQRT(1/30*SUM(L52:M52,P52,Q52,S52))</f>
+        <v>9.7109968865731672E-2</v>
       </c>
     </row>
     <row r="62" spans="2:24" x14ac:dyDescent="0.25">
@@ -5147,7 +5162,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDD4079C-107F-47DA-884D-859E342E8E03}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
timon mag puschie pushie
</commit_message>
<xml_diff>
--- a/B 2.2/Messdaten/Auswertungsskripte/B2.2.xlsx
+++ b/B 2.2/Messdaten/Auswertungsskripte/B2.2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dtimo\Desktop\Praktikum\praktikum\B 2.2\Messdaten\Auswertungsskripte\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesco\Documents\Praktikum-test\B 2.2\Messdaten\Auswertungsskripte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209F8386-F17F-4440-9914-DD2BD0AB645C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{158E7B65-4E26-488F-93BA-6827F689EBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="54">
   <si>
     <t>s</t>
   </si>
@@ -163,6 +163,42 @@
   <si>
     <t>S^2-S</t>
   </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>dr</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>db</t>
+  </si>
+  <si>
+    <t>dl</t>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>dA</t>
+  </si>
+  <si>
+    <t>dp</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>dS</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
 </sst>
 </file>
 
@@ -171,10 +207,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -224,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -232,13 +274,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -521,7 +564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:BA57"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -3067,7 +3110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{540561B1-14D7-4856-AC05-2802599319CD}">
   <dimension ref="B4:X68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+    <sheetView topLeftCell="B22" workbookViewId="0">
       <selection activeCell="O55" sqref="O55"/>
     </sheetView>
   </sheetViews>
@@ -3077,16 +3120,16 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
@@ -3192,7 +3235,7 @@
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C7">
@@ -3254,7 +3297,7 @@
       </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B8" s="7"/>
+      <c r="B8" s="8"/>
       <c r="C8">
         <v>71.36</v>
       </c>
@@ -3314,7 +3357,7 @@
       </c>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B9" s="7"/>
+      <c r="B9" s="8"/>
       <c r="C9">
         <v>86.2</v>
       </c>
@@ -3374,7 +3417,7 @@
       </c>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
+      <c r="B10" s="8"/>
       <c r="C10">
         <v>91.02</v>
       </c>
@@ -4081,16 +4124,16 @@
       </c>
     </row>
     <row r="37" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
@@ -4131,7 +4174,7 @@
       <c r="V38" s="5"/>
     </row>
     <row r="39" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C39">
@@ -4190,7 +4233,7 @@
       </c>
     </row>
     <row r="40" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B40" s="7"/>
+      <c r="B40" s="8"/>
       <c r="C40">
         <v>71.08</v>
       </c>
@@ -4247,7 +4290,7 @@
       </c>
     </row>
     <row r="41" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B41" s="7"/>
+      <c r="B41" s="8"/>
       <c r="C41">
         <v>85.98</v>
       </c>
@@ -4305,7 +4348,7 @@
       </c>
     </row>
     <row r="42" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B42" s="7"/>
+      <c r="B42" s="8"/>
       <c r="C42">
         <v>90.5</v>
       </c>
@@ -4989,7 +5032,7 @@
         <f>AVERAGE(L51:M51,P51:Q51,S51:T51,W51)</f>
         <v>0.38727533215341853</v>
       </c>
-      <c r="M53" s="9">
+      <c r="M53" s="7">
         <f>AVERAGE(L51:M51,P51:Q51,S51:T51)</f>
         <v>0.17569823989767314</v>
       </c>
@@ -5002,22 +5045,22 @@
         <f>SQRT(1/30*SUM(L52:M52,P52,Q52,S52,W52))</f>
         <v>0.21618140767867511</v>
       </c>
-      <c r="M54" s="9">
+      <c r="M54" s="7">
         <f>SQRT(1/30*SUM(L52:M52,P52,Q52,S52))</f>
         <v>9.7109968865731672E-2</v>
       </c>
     </row>
     <row r="62" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B62" s="8" t="s">
+      <c r="B62" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
-      <c r="F62" s="8"/>
-      <c r="G62" s="8"/>
-      <c r="H62" s="8"/>
-      <c r="I62" s="8"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9"/>
+      <c r="H62" s="9"/>
+      <c r="I62" s="9"/>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
       <c r="L62" s="4"/>
@@ -5053,7 +5096,7 @@
       </c>
     </row>
     <row r="64" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B64" s="7" t="s">
+      <c r="B64" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C64">
@@ -5073,7 +5116,7 @@
       </c>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B65" s="7"/>
+      <c r="B65" s="8"/>
       <c r="C65">
         <v>68.88</v>
       </c>
@@ -5094,7 +5137,7 @@
       </c>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B66" s="7"/>
+      <c r="B66" s="8"/>
       <c r="C66">
         <v>82.9</v>
       </c>
@@ -5115,7 +5158,7 @@
       </c>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B67" s="7"/>
+      <c r="B67" s="8"/>
       <c r="C67">
         <v>87.6</v>
       </c>
@@ -5160,14 +5203,222 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDD4079C-107F-47DA-884D-859E342E8E03}">
-  <dimension ref="A1"/>
+  <dimension ref="F2:Q14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" s="10">
+        <v>3.8999999999999999E-4</v>
+      </c>
+      <c r="H3" s="10">
+        <v>9.9000000000000005E-7</v>
+      </c>
+      <c r="I3" s="10">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="J3" s="10">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="K3" s="10">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="L3" s="10">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="M3" s="10">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="N3" s="10">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="P3">
+        <f>SQRT((J3*M3*G3/K3)^2+(I3*G3*N3/K3)^2+(I3*M3*H3/K3)^2+(I3*M3*G3*L3/K3^2)^2)</f>
+        <v>1.4854766364107948E-8</v>
+      </c>
+      <c r="Q3" s="10">
+        <f>I3*M3*G3/K3</f>
+        <v>5.937313432835822E-8</v>
+      </c>
+    </row>
+    <row r="4" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4" s="10">
+        <v>2.5999999999999998E-4</v>
+      </c>
+      <c r="H4" s="10">
+        <v>1.5E-6</v>
+      </c>
+      <c r="I4" s="10">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="J4" s="10">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="K4" s="10">
+        <v>4.3E-3</v>
+      </c>
+      <c r="L4" s="10">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="M4" s="10">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="N4" s="10">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4:P5" si="0">SQRT((J4*M4*G4/K4)^2+(I4*G4*N4/K4)^2+(I4*M4*H4/K4)^2+(I4*M4*G4*L4/K4^2)^2)</f>
+        <v>1.5746286668795033E-8</v>
+      </c>
+      <c r="Q4" s="10">
+        <f t="shared" ref="Q4:Q5" si="1">I4*M4*G4/K4</f>
+        <v>6.2883720930232546E-8</v>
+      </c>
+    </row>
+    <row r="5" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5" s="10">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="H5" s="10">
+        <v>9.0999999999999997E-7</v>
+      </c>
+      <c r="I5" s="10">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="J5" s="10">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="K5" s="10">
+        <v>4.1000000000000003E-3</v>
+      </c>
+      <c r="L5" s="10">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="M5" s="10">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="N5" s="10">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>1.6194445912481182E-7</v>
+      </c>
+      <c r="Q5" s="10">
+        <f t="shared" si="1"/>
+        <v>6.4682926829268299E-7</v>
+      </c>
+    </row>
+    <row r="10" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10">
+        <f>(P5-P3)/(0.25*0.75)</f>
+        <v>7.844783613904207E-7</v>
+      </c>
+      <c r="I10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10">
+        <f>SQRT((Q5-Q4)/(Q5-Q3))</f>
+        <v>0.99700756629453469</v>
+      </c>
+    </row>
+    <row r="11" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11">
+        <f>1/(0.25*0.75) * SQRT(P5^2+P3^2)</f>
+        <v>8.6732974716077602E-7</v>
+      </c>
+      <c r="I11" t="s">
+        <v>52</v>
+      </c>
+      <c r="J11">
+        <f>SQRT(J12+J13+J14)</f>
+        <v>1.8446578725678169E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>5</v>
+      </c>
+      <c r="J12" s="10">
+        <f>(1/(2*J10*(Q5-Q3)) * P4)^2</f>
+        <v>1.806959929807293E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>44</v>
+      </c>
+      <c r="J13" s="10">
+        <f>((Q5-Q4)*P3/(2*J10*(Q5-Q3)^2))^2</f>
+        <v>1.5889772617479485E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>53</v>
+      </c>
+      <c r="J14" s="10">
+        <f>(P5*(Q4-Q3)/(J10*2*(Q5-Q3)^2))^2</f>
+        <v>6.8254752711828959E-7</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>